<commit_message>
fixing formula for the teamrating
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lazarekolebka/Documents/GitHub/baby-foot-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5716B55B-A467-8747-B06E-A4C8B0DCFB72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBBAD07-922A-8747-9D6E-6591CE36F320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16520" xr2:uid="{3047FE35-D3D7-B143-93A4-201EEA00FB6B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4160" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4380" uniqueCount="21">
   <si>
     <t>Lazare</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Yassine</t>
+  </si>
+  <si>
+    <t>NathanD</t>
   </si>
 </sst>
 </file>
@@ -466,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8CBF0B-E51F-9843-B378-4476707EC7F4}">
-  <dimension ref="A1:H1506"/>
+  <dimension ref="A1:Z1504"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:G23"/>
+    <sheetView tabSelected="1" topLeftCell="A844" workbookViewId="0">
+      <selection activeCell="D861" sqref="D861"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28125,7 +28128,7 @@
         <v>ok</v>
       </c>
     </row>
-    <row r="1025" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1025" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1025" s="1">
         <v>44952.556701388887</v>
       </c>
@@ -28152,7 +28155,7 @@
         <v>ok</v>
       </c>
     </row>
-    <row r="1026" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1026" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1026" s="1">
         <v>44953.546678240738</v>
       </c>
@@ -28175,11 +28178,11 @@
         <v>11</v>
       </c>
       <c r="H1026" t="str">
-        <f t="shared" ref="H1026:H1040" si="16">IF(D1026=G1026,"error","ok")</f>
-        <v>ok</v>
-      </c>
-    </row>
-    <row r="1027" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ref="H1026:H1089" si="16">IF(D1026=G1026,"error","ok")</f>
+        <v>ok</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1027" s="1">
         <v>44953.552824074075</v>
       </c>
@@ -28206,7 +28209,7 @@
         <v>ok</v>
       </c>
     </row>
-    <row r="1028" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1028" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1028" s="1">
         <v>44953.669849537036</v>
       </c>
@@ -28233,7 +28236,7 @@
         <v>ok</v>
       </c>
     </row>
-    <row r="1029" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1029" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1029" s="1">
         <v>44953.675324074073</v>
       </c>
@@ -28260,7 +28263,7 @@
         <v>ok</v>
       </c>
     </row>
-    <row r="1030" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1030" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1030" s="1">
         <v>44953.679340277777</v>
       </c>
@@ -28287,7 +28290,7 @@
         <v>ok</v>
       </c>
     </row>
-    <row r="1031" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1031" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1031" s="1">
         <v>44954.668379629627</v>
       </c>
@@ -28314,7 +28317,7 @@
         <v>ok</v>
       </c>
     </row>
-    <row r="1032" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1032" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1032" s="1">
         <v>44956.529756944445</v>
       </c>
@@ -28341,7 +28344,7 @@
         <v>ok</v>
       </c>
     </row>
-    <row r="1033" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1033" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1033" s="1">
         <v>44956.683599537035</v>
       </c>
@@ -28368,7 +28371,7 @@
         <v>ok</v>
       </c>
     </row>
-    <row r="1034" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1034" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1034" s="1">
         <v>44957.533437500002</v>
       </c>
@@ -28395,7 +28398,7 @@
         <v>ok</v>
       </c>
     </row>
-    <row r="1035" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1035" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1035" s="1">
         <v>44957.54351851852</v>
       </c>
@@ -28422,7 +28425,7 @@
         <v>ok</v>
       </c>
     </row>
-    <row r="1036" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1036" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1036" s="1">
         <v>44957.55127314815</v>
       </c>
@@ -28449,7 +28452,7 @@
         <v>ok</v>
       </c>
     </row>
-    <row r="1037" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1037" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1037" s="1">
         <v>44957.677523148152</v>
       </c>
@@ -28476,7 +28479,7 @@
         <v>ok</v>
       </c>
     </row>
-    <row r="1038" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1038" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1038" s="1">
         <v>44957.691504629627</v>
       </c>
@@ -28503,12 +28506,12 @@
         <v>ok</v>
       </c>
     </row>
-    <row r="1039" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1039" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1039" s="1">
-        <v>44960.66505787037</v>
+        <v>44959.541643518518</v>
       </c>
       <c r="B1039" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1039" s="2" t="s">
         <v>17</v>
@@ -28517,542 +28520,2557 @@
         <v>11</v>
       </c>
       <c r="E1039" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F1039" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G1039" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H1039" t="str">
         <f t="shared" si="16"/>
         <v>ok</v>
       </c>
-    </row>
-    <row r="1040" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1039" s="2"/>
+      <c r="J1039" s="2"/>
+      <c r="K1039" s="2"/>
+      <c r="L1039" s="2"/>
+      <c r="M1039" s="2"/>
+      <c r="N1039" s="2"/>
+      <c r="O1039" s="2"/>
+      <c r="P1039" s="2"/>
+      <c r="Q1039" s="2"/>
+      <c r="R1039" s="2"/>
+      <c r="S1039" s="2"/>
+      <c r="T1039" s="2"/>
+      <c r="U1039" s="2"/>
+      <c r="V1039" s="2"/>
+      <c r="W1039" s="2"/>
+      <c r="X1039" s="2"/>
+      <c r="Y1039" s="2"/>
+      <c r="Z1039" s="2"/>
+    </row>
+    <row r="1040" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1040" s="1">
-        <v>44960.67460648148</v>
+        <v>44959.542129629626</v>
       </c>
       <c r="B1040" s="2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C1040" s="2" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D1040" s="2">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E1040" s="2" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F1040" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G1040" s="2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H1040" t="str">
         <f t="shared" si="16"/>
         <v>ok</v>
       </c>
-    </row>
-    <row r="1041" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1041" s="2"/>
-      <c r="B1041" s="2"/>
-      <c r="C1041" s="2"/>
-      <c r="D1041" s="2"/>
-      <c r="E1041" s="2"/>
-      <c r="F1041" s="2"/>
-      <c r="G1041" s="2"/>
-    </row>
-    <row r="1042" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1042" s="2"/>
-      <c r="B1042" s="2"/>
-      <c r="C1042" s="2"/>
-      <c r="D1042" s="2"/>
-      <c r="E1042" s="2"/>
-      <c r="F1042" s="2"/>
-      <c r="G1042" s="2"/>
-    </row>
-    <row r="1043" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1043" s="2"/>
-      <c r="B1043" s="2"/>
-      <c r="C1043" s="2"/>
-      <c r="D1043" s="2"/>
-      <c r="E1043" s="2"/>
-      <c r="F1043" s="2"/>
-      <c r="G1043" s="2"/>
-    </row>
-    <row r="1044" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1044" s="2"/>
-      <c r="B1044" s="2"/>
-      <c r="C1044" s="2"/>
-      <c r="D1044" s="2"/>
-      <c r="E1044" s="2"/>
-      <c r="F1044" s="2"/>
-      <c r="G1044" s="2"/>
-    </row>
-    <row r="1045" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1045" s="2"/>
-      <c r="B1045" s="2"/>
-      <c r="C1045" s="2"/>
-      <c r="D1045" s="2"/>
-      <c r="E1045" s="2"/>
-      <c r="F1045" s="2"/>
-      <c r="G1045" s="2"/>
-    </row>
-    <row r="1046" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1046" s="2"/>
-      <c r="B1046" s="2"/>
-      <c r="C1046" s="2"/>
-      <c r="D1046" s="2"/>
-      <c r="E1046" s="2"/>
-      <c r="F1046" s="2"/>
-      <c r="G1046" s="2"/>
-    </row>
-    <row r="1047" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1047" s="2"/>
-      <c r="B1047" s="2"/>
-      <c r="C1047" s="2"/>
-      <c r="D1047" s="2"/>
-      <c r="E1047" s="2"/>
-      <c r="F1047" s="2"/>
-      <c r="G1047" s="2"/>
-    </row>
-    <row r="1048" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1048" s="2"/>
-      <c r="B1048" s="2"/>
-      <c r="C1048" s="2"/>
-      <c r="D1048" s="2"/>
-      <c r="E1048" s="2"/>
-      <c r="F1048" s="2"/>
-      <c r="G1048" s="2"/>
-    </row>
-    <row r="1049" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1049" s="2"/>
-      <c r="B1049" s="2"/>
-      <c r="C1049" s="2"/>
-      <c r="D1049" s="2"/>
-      <c r="E1049" s="2"/>
-      <c r="F1049" s="2"/>
-      <c r="G1049" s="2"/>
-    </row>
-    <row r="1050" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1050" s="2"/>
-      <c r="B1050" s="2"/>
-      <c r="C1050" s="2"/>
-      <c r="D1050" s="2"/>
-      <c r="E1050" s="2"/>
-      <c r="F1050" s="2"/>
-      <c r="G1050" s="2"/>
-    </row>
-    <row r="1051" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1051" s="2"/>
-      <c r="B1051" s="2"/>
-      <c r="C1051" s="2"/>
-      <c r="D1051" s="2"/>
-      <c r="E1051" s="2"/>
-      <c r="F1051" s="2"/>
-      <c r="G1051" s="2"/>
-    </row>
-    <row r="1052" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1052" s="2"/>
-      <c r="B1052" s="2"/>
-      <c r="C1052" s="2"/>
-      <c r="D1052" s="2"/>
-      <c r="E1052" s="2"/>
-      <c r="F1052" s="2"/>
-      <c r="G1052" s="2"/>
-    </row>
-    <row r="1053" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1053" s="2"/>
-      <c r="B1053" s="2"/>
-      <c r="C1053" s="2"/>
-      <c r="D1053" s="2"/>
-      <c r="E1053" s="2"/>
-      <c r="F1053" s="2"/>
-      <c r="G1053" s="2"/>
-    </row>
-    <row r="1054" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1054" s="2"/>
-      <c r="B1054" s="2"/>
-      <c r="C1054" s="2"/>
-      <c r="D1054" s="2"/>
-      <c r="E1054" s="2"/>
-      <c r="F1054" s="2"/>
-      <c r="G1054" s="2"/>
-    </row>
-    <row r="1055" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1055" s="2"/>
-      <c r="B1055" s="2"/>
-      <c r="C1055" s="2"/>
-      <c r="D1055" s="2"/>
-      <c r="E1055" s="2"/>
-      <c r="F1055" s="2"/>
-      <c r="G1055" s="2"/>
-    </row>
-    <row r="1056" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1056" s="2"/>
-      <c r="B1056" s="2"/>
-      <c r="C1056" s="2"/>
-      <c r="D1056" s="2"/>
-      <c r="E1056" s="2"/>
-      <c r="F1056" s="2"/>
-      <c r="G1056" s="2"/>
-    </row>
-    <row r="1057" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1057" s="2"/>
-      <c r="B1057" s="2"/>
-      <c r="C1057" s="2"/>
-      <c r="D1057" s="2"/>
-      <c r="E1057" s="2"/>
-      <c r="F1057" s="2"/>
-      <c r="G1057" s="2"/>
-    </row>
-    <row r="1058" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1058" s="2"/>
-      <c r="B1058" s="2"/>
-      <c r="C1058" s="2"/>
-      <c r="D1058" s="2"/>
-      <c r="E1058" s="2"/>
-      <c r="F1058" s="2"/>
-      <c r="G1058" s="2"/>
-    </row>
-    <row r="1059" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1059" s="2"/>
-      <c r="B1059" s="2"/>
-      <c r="C1059" s="2"/>
-      <c r="D1059" s="2"/>
-      <c r="E1059" s="2"/>
-      <c r="F1059" s="2"/>
-      <c r="G1059" s="2"/>
-    </row>
-    <row r="1060" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1060" s="2"/>
-      <c r="B1060" s="2"/>
-      <c r="C1060" s="2"/>
-      <c r="D1060" s="2"/>
-      <c r="E1060" s="2"/>
-      <c r="F1060" s="2"/>
-      <c r="G1060" s="2"/>
-    </row>
-    <row r="1061" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1061" s="2"/>
-      <c r="B1061" s="2"/>
-      <c r="C1061" s="2"/>
-      <c r="D1061" s="2"/>
-      <c r="E1061" s="2"/>
-      <c r="F1061" s="2"/>
-      <c r="G1061" s="2"/>
-    </row>
-    <row r="1062" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1062" s="2"/>
-      <c r="B1062" s="2"/>
-      <c r="C1062" s="2"/>
-      <c r="D1062" s="2"/>
-      <c r="E1062" s="2"/>
-      <c r="F1062" s="2"/>
-      <c r="G1062" s="2"/>
-    </row>
-    <row r="1063" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1063" s="2"/>
-      <c r="B1063" s="2"/>
-      <c r="C1063" s="2"/>
-      <c r="D1063" s="2"/>
-      <c r="E1063" s="2"/>
-      <c r="F1063" s="2"/>
-      <c r="G1063" s="2"/>
-    </row>
-    <row r="1064" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1064" s="2"/>
-      <c r="B1064" s="2"/>
-      <c r="C1064" s="2"/>
-      <c r="D1064" s="2"/>
-      <c r="E1064" s="2"/>
-      <c r="F1064" s="2"/>
-      <c r="G1064" s="2"/>
-    </row>
-    <row r="1065" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1065" s="2"/>
-      <c r="B1065" s="2"/>
-      <c r="C1065" s="2"/>
-      <c r="D1065" s="2"/>
-      <c r="E1065" s="2"/>
-      <c r="F1065" s="2"/>
-      <c r="G1065" s="2"/>
-    </row>
-    <row r="1066" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1066" s="2"/>
-      <c r="B1066" s="2"/>
-      <c r="C1066" s="2"/>
-      <c r="D1066" s="2"/>
-      <c r="E1066" s="2"/>
-      <c r="F1066" s="2"/>
-      <c r="G1066" s="2"/>
-    </row>
-    <row r="1067" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1067" s="2"/>
-      <c r="B1067" s="2"/>
-      <c r="C1067" s="2"/>
-      <c r="D1067" s="2"/>
-      <c r="E1067" s="2"/>
-      <c r="F1067" s="2"/>
-      <c r="G1067" s="2"/>
-    </row>
-    <row r="1068" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1068" s="2"/>
-      <c r="B1068" s="2"/>
-      <c r="C1068" s="2"/>
-      <c r="D1068" s="2"/>
-      <c r="E1068" s="2"/>
-      <c r="F1068" s="2"/>
-      <c r="G1068" s="2"/>
-    </row>
-    <row r="1069" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1069" s="2"/>
-      <c r="B1069" s="2"/>
-      <c r="C1069" s="2"/>
-      <c r="D1069" s="2"/>
-      <c r="E1069" s="2"/>
-      <c r="F1069" s="2"/>
-      <c r="G1069" s="2"/>
-    </row>
-    <row r="1070" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1070" s="2"/>
-      <c r="B1070" s="2"/>
-      <c r="C1070" s="2"/>
-      <c r="D1070" s="2"/>
-      <c r="E1070" s="2"/>
-      <c r="F1070" s="2"/>
-      <c r="G1070" s="2"/>
-    </row>
-    <row r="1071" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1071" s="2"/>
-      <c r="B1071" s="2"/>
-      <c r="C1071" s="2"/>
-      <c r="D1071" s="2"/>
-      <c r="E1071" s="2"/>
-      <c r="F1071" s="2"/>
-      <c r="G1071" s="2"/>
-    </row>
-    <row r="1072" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1072" s="2"/>
-      <c r="B1072" s="2"/>
-      <c r="C1072" s="2"/>
-      <c r="D1072" s="2"/>
-      <c r="E1072" s="2"/>
-      <c r="F1072" s="2"/>
-      <c r="G1072" s="2"/>
-    </row>
-    <row r="1073" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1073" s="2"/>
-      <c r="B1073" s="2"/>
-      <c r="C1073" s="2"/>
-      <c r="D1073" s="2"/>
-      <c r="E1073" s="2"/>
-      <c r="F1073" s="2"/>
-      <c r="G1073" s="2"/>
-    </row>
-    <row r="1074" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1074" s="2"/>
-      <c r="B1074" s="2"/>
-      <c r="C1074" s="2"/>
-      <c r="D1074" s="2"/>
-      <c r="E1074" s="2"/>
-      <c r="F1074" s="2"/>
-      <c r="G1074" s="2"/>
-    </row>
-    <row r="1075" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1075" s="2"/>
-      <c r="B1075" s="2"/>
-      <c r="C1075" s="2"/>
-      <c r="D1075" s="2"/>
-      <c r="E1075" s="2"/>
-      <c r="F1075" s="2"/>
-      <c r="G1075" s="2"/>
-    </row>
-    <row r="1076" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1076" s="2"/>
-      <c r="B1076" s="2"/>
-      <c r="C1076" s="2"/>
-      <c r="D1076" s="2"/>
-      <c r="E1076" s="2"/>
-      <c r="F1076" s="2"/>
-      <c r="G1076" s="2"/>
-    </row>
-    <row r="1077" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1077" s="2"/>
-      <c r="B1077" s="2"/>
-      <c r="C1077" s="2"/>
-      <c r="D1077" s="2"/>
-      <c r="E1077" s="2"/>
-      <c r="F1077" s="2"/>
-      <c r="G1077" s="2"/>
-    </row>
-    <row r="1078" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1078" s="2"/>
-      <c r="B1078" s="2"/>
-      <c r="C1078" s="2"/>
-      <c r="D1078" s="2"/>
-      <c r="E1078" s="2"/>
-      <c r="F1078" s="2"/>
-      <c r="G1078" s="2"/>
-    </row>
-    <row r="1079" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1079" s="2"/>
-      <c r="B1079" s="2"/>
-      <c r="C1079" s="2"/>
-      <c r="D1079" s="2"/>
-      <c r="E1079" s="2"/>
-      <c r="F1079" s="2"/>
-      <c r="G1079" s="2"/>
-    </row>
-    <row r="1080" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1080" s="2"/>
-      <c r="B1080" s="2"/>
-      <c r="C1080" s="2"/>
-      <c r="D1080" s="2"/>
-      <c r="E1080" s="2"/>
-      <c r="F1080" s="2"/>
-      <c r="G1080" s="2"/>
-    </row>
-    <row r="1081" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1081" s="2"/>
-      <c r="B1081" s="2"/>
-      <c r="C1081" s="2"/>
-      <c r="D1081" s="2"/>
-      <c r="E1081" s="2"/>
-      <c r="F1081" s="2"/>
-      <c r="G1081" s="2"/>
-    </row>
-    <row r="1082" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1082" s="2"/>
-      <c r="B1082" s="2"/>
-      <c r="C1082" s="2"/>
-      <c r="D1082" s="2"/>
-      <c r="E1082" s="2"/>
-      <c r="F1082" s="2"/>
-      <c r="G1082" s="2"/>
-    </row>
-    <row r="1083" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1083" s="2"/>
-      <c r="B1083" s="2"/>
-      <c r="C1083" s="2"/>
-      <c r="D1083" s="2"/>
-      <c r="E1083" s="2"/>
-      <c r="F1083" s="2"/>
-      <c r="G1083" s="2"/>
-    </row>
-    <row r="1084" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1084" s="2"/>
-      <c r="B1084" s="2"/>
-      <c r="C1084" s="2"/>
-      <c r="D1084" s="2"/>
-      <c r="E1084" s="2"/>
-      <c r="F1084" s="2"/>
-      <c r="G1084" s="2"/>
-    </row>
-    <row r="1085" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1085" s="2"/>
-      <c r="B1085" s="2"/>
-      <c r="C1085" s="2"/>
-      <c r="D1085" s="2"/>
-      <c r="E1085" s="2"/>
-      <c r="F1085" s="2"/>
-      <c r="G1085" s="2"/>
-    </row>
-    <row r="1086" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1086" s="2"/>
-      <c r="B1086" s="2"/>
-      <c r="C1086" s="2"/>
-      <c r="D1086" s="2"/>
-      <c r="E1086" s="2"/>
-      <c r="F1086" s="2"/>
-      <c r="G1086" s="2"/>
-    </row>
-    <row r="1087" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1087" s="2"/>
-      <c r="B1087" s="2"/>
-      <c r="C1087" s="2"/>
-      <c r="D1087" s="2"/>
-      <c r="E1087" s="2"/>
-      <c r="F1087" s="2"/>
-      <c r="G1087" s="2"/>
-    </row>
-    <row r="1088" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1088" s="2"/>
-      <c r="B1088" s="2"/>
-      <c r="C1088" s="2"/>
-      <c r="D1088" s="2"/>
-      <c r="E1088" s="2"/>
-      <c r="F1088" s="2"/>
-      <c r="G1088" s="2"/>
-    </row>
-    <row r="1089" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1089" s="2"/>
-      <c r="B1089" s="2"/>
-      <c r="C1089" s="2"/>
-      <c r="D1089" s="2"/>
-      <c r="E1089" s="2"/>
-      <c r="F1089" s="2"/>
-      <c r="G1089" s="2"/>
-    </row>
-    <row r="1090" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1090" s="2"/>
-      <c r="B1090" s="2"/>
-      <c r="C1090" s="2"/>
-      <c r="D1090" s="2"/>
-      <c r="E1090" s="2"/>
-      <c r="F1090" s="2"/>
-      <c r="G1090" s="2"/>
-    </row>
-    <row r="1091" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1091" s="2"/>
-      <c r="B1091" s="2"/>
-      <c r="C1091" s="2"/>
-      <c r="D1091" s="2"/>
-      <c r="E1091" s="2"/>
-      <c r="F1091" s="2"/>
-      <c r="G1091" s="2"/>
-    </row>
-    <row r="1092" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1092" s="2"/>
-      <c r="B1092" s="2"/>
-      <c r="C1092" s="2"/>
-      <c r="D1092" s="2"/>
-      <c r="E1092" s="2"/>
-      <c r="F1092" s="2"/>
-      <c r="G1092" s="2"/>
-    </row>
-    <row r="1093" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1093" s="2"/>
-      <c r="B1093" s="2"/>
-      <c r="C1093" s="2"/>
-      <c r="D1093" s="2"/>
-      <c r="E1093" s="2"/>
-      <c r="F1093" s="2"/>
-      <c r="G1093" s="2"/>
-    </row>
-    <row r="1094" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1094" s="2"/>
-      <c r="B1094" s="2"/>
-      <c r="C1094" s="2"/>
-      <c r="D1094" s="2"/>
-      <c r="E1094" s="2"/>
-      <c r="F1094" s="2"/>
-      <c r="G1094" s="2"/>
-    </row>
-    <row r="1095" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1095" s="2"/>
-      <c r="B1095" s="2"/>
-      <c r="C1095" s="2"/>
-      <c r="D1095" s="2"/>
-      <c r="E1095" s="2"/>
-      <c r="F1095" s="2"/>
-      <c r="G1095" s="2"/>
-    </row>
-    <row r="1096" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I1040" s="2"/>
+      <c r="J1040" s="2"/>
+      <c r="K1040" s="2"/>
+      <c r="L1040" s="2"/>
+      <c r="M1040" s="2"/>
+      <c r="N1040" s="2"/>
+      <c r="O1040" s="2"/>
+      <c r="P1040" s="2"/>
+      <c r="Q1040" s="2"/>
+      <c r="R1040" s="2"/>
+      <c r="S1040" s="2"/>
+      <c r="T1040" s="2"/>
+      <c r="U1040" s="2"/>
+      <c r="V1040" s="2"/>
+      <c r="W1040" s="2"/>
+      <c r="X1040" s="2"/>
+      <c r="Y1040" s="2"/>
+      <c r="Z1040" s="2"/>
+    </row>
+    <row r="1041" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1041" s="1">
+        <v>44959.552465277775</v>
+      </c>
+      <c r="B1041" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1041" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1041" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1041" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1041" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1041" s="2">
+        <v>8</v>
+      </c>
+      <c r="H1041" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1041" s="2"/>
+      <c r="J1041" s="2"/>
+      <c r="K1041" s="2"/>
+      <c r="L1041" s="2"/>
+      <c r="M1041" s="2"/>
+      <c r="N1041" s="2"/>
+      <c r="O1041" s="2"/>
+      <c r="P1041" s="2"/>
+      <c r="Q1041" s="2"/>
+      <c r="R1041" s="2"/>
+      <c r="S1041" s="2"/>
+      <c r="T1041" s="2"/>
+      <c r="U1041" s="2"/>
+      <c r="V1041" s="2"/>
+      <c r="W1041" s="2"/>
+      <c r="X1041" s="2"/>
+      <c r="Y1041" s="2"/>
+      <c r="Z1041" s="2"/>
+    </row>
+    <row r="1042" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1042" s="1">
+        <v>44959.695856481485</v>
+      </c>
+      <c r="B1042" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1042" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1042" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1042" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1042" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1042" s="2">
+        <v>5</v>
+      </c>
+      <c r="H1042" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1042" s="2"/>
+      <c r="J1042" s="2"/>
+      <c r="K1042" s="2"/>
+      <c r="L1042" s="2"/>
+      <c r="M1042" s="2"/>
+      <c r="N1042" s="2"/>
+      <c r="O1042" s="2"/>
+      <c r="P1042" s="2"/>
+      <c r="Q1042" s="2"/>
+      <c r="R1042" s="2"/>
+      <c r="S1042" s="2"/>
+      <c r="T1042" s="2"/>
+      <c r="U1042" s="2"/>
+      <c r="V1042" s="2"/>
+      <c r="W1042" s="2"/>
+      <c r="X1042" s="2"/>
+      <c r="Y1042" s="2"/>
+      <c r="Z1042" s="2"/>
+    </row>
+    <row r="1043" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1043" s="1">
+        <v>44959.71603009259</v>
+      </c>
+      <c r="B1043" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1043" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1043" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1043" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1043" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1043" s="2">
+        <v>3</v>
+      </c>
+      <c r="H1043" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1043" s="2"/>
+      <c r="J1043" s="2"/>
+      <c r="K1043" s="2"/>
+      <c r="L1043" s="2"/>
+      <c r="M1043" s="2"/>
+      <c r="N1043" s="2"/>
+      <c r="O1043" s="2"/>
+      <c r="P1043" s="2"/>
+      <c r="Q1043" s="2"/>
+      <c r="R1043" s="2"/>
+      <c r="S1043" s="2"/>
+      <c r="T1043" s="2"/>
+      <c r="U1043" s="2"/>
+      <c r="V1043" s="2"/>
+      <c r="W1043" s="2"/>
+      <c r="X1043" s="2"/>
+      <c r="Y1043" s="2"/>
+      <c r="Z1043" s="2"/>
+    </row>
+    <row r="1044" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1044" s="1">
+        <v>44960.66505787037</v>
+      </c>
+      <c r="B1044" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1044" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1044" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1044" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1044" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1044" s="2">
+        <v>5</v>
+      </c>
+      <c r="H1044" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1044" s="2"/>
+      <c r="J1044" s="2"/>
+      <c r="K1044" s="2"/>
+      <c r="L1044" s="2"/>
+      <c r="M1044" s="2"/>
+      <c r="N1044" s="2"/>
+      <c r="O1044" s="2"/>
+      <c r="P1044" s="2"/>
+      <c r="Q1044" s="2"/>
+      <c r="R1044" s="2"/>
+      <c r="S1044" s="2"/>
+      <c r="T1044" s="2"/>
+      <c r="U1044" s="2"/>
+      <c r="V1044" s="2"/>
+      <c r="W1044" s="2"/>
+      <c r="X1044" s="2"/>
+      <c r="Y1044" s="2"/>
+      <c r="Z1044" s="2"/>
+    </row>
+    <row r="1045" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1045" s="1">
+        <v>44960.67460648148</v>
+      </c>
+      <c r="B1045" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1045" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1045" s="2">
+        <v>6</v>
+      </c>
+      <c r="E1045" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1045" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1045" s="2">
+        <v>11</v>
+      </c>
+      <c r="H1045" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1045" s="2"/>
+      <c r="J1045" s="2"/>
+      <c r="K1045" s="2"/>
+      <c r="L1045" s="2"/>
+      <c r="M1045" s="2"/>
+      <c r="N1045" s="2"/>
+      <c r="O1045" s="2"/>
+      <c r="P1045" s="2"/>
+      <c r="Q1045" s="2"/>
+      <c r="R1045" s="2"/>
+      <c r="S1045" s="2"/>
+      <c r="T1045" s="2"/>
+      <c r="U1045" s="2"/>
+      <c r="V1045" s="2"/>
+      <c r="W1045" s="2"/>
+      <c r="X1045" s="2"/>
+      <c r="Y1045" s="2"/>
+      <c r="Z1045" s="2"/>
+    </row>
+    <row r="1046" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1046" s="1">
+        <v>44963.525810185187</v>
+      </c>
+      <c r="B1046" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1046" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1046" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1046" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1046" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1046" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1046" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1046" s="2"/>
+      <c r="J1046" s="2"/>
+      <c r="K1046" s="2"/>
+      <c r="L1046" s="2"/>
+      <c r="M1046" s="2"/>
+      <c r="N1046" s="2"/>
+      <c r="O1046" s="2"/>
+      <c r="P1046" s="2"/>
+      <c r="Q1046" s="2"/>
+      <c r="R1046" s="2"/>
+      <c r="S1046" s="2"/>
+      <c r="T1046" s="2"/>
+      <c r="U1046" s="2"/>
+      <c r="V1046" s="2"/>
+      <c r="W1046" s="2"/>
+      <c r="X1046" s="2"/>
+      <c r="Y1046" s="2"/>
+      <c r="Z1046" s="2"/>
+    </row>
+    <row r="1047" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1047" s="1">
+        <v>44963.54420138889</v>
+      </c>
+      <c r="B1047" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1047" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1047" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1047" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1047" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1047" s="2">
+        <v>4</v>
+      </c>
+      <c r="H1047" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1047" s="2"/>
+      <c r="J1047" s="2"/>
+      <c r="K1047" s="2"/>
+      <c r="L1047" s="2"/>
+      <c r="M1047" s="2"/>
+      <c r="N1047" s="2"/>
+      <c r="O1047" s="2"/>
+      <c r="P1047" s="2"/>
+      <c r="Q1047" s="2"/>
+      <c r="R1047" s="2"/>
+      <c r="S1047" s="2"/>
+      <c r="T1047" s="2"/>
+      <c r="U1047" s="2"/>
+      <c r="V1047" s="2"/>
+      <c r="W1047" s="2"/>
+      <c r="X1047" s="2"/>
+      <c r="Y1047" s="2"/>
+      <c r="Z1047" s="2"/>
+    </row>
+    <row r="1048" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1048" s="1">
+        <v>44963.556898148148</v>
+      </c>
+      <c r="B1048" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1048" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1048" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1048" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1048" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1048" s="2">
+        <v>4</v>
+      </c>
+      <c r="H1048" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1048" s="2"/>
+      <c r="J1048" s="2"/>
+      <c r="K1048" s="2"/>
+      <c r="L1048" s="2"/>
+      <c r="M1048" s="2"/>
+      <c r="N1048" s="2"/>
+      <c r="O1048" s="2"/>
+      <c r="P1048" s="2"/>
+      <c r="Q1048" s="2"/>
+      <c r="R1048" s="2"/>
+      <c r="S1048" s="2"/>
+      <c r="T1048" s="2"/>
+      <c r="U1048" s="2"/>
+      <c r="V1048" s="2"/>
+      <c r="W1048" s="2"/>
+      <c r="X1048" s="2"/>
+      <c r="Y1048" s="2"/>
+      <c r="Z1048" s="2"/>
+    </row>
+    <row r="1049" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1049" s="1">
+        <v>44963.68105324074</v>
+      </c>
+      <c r="B1049" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1049" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1049" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1049" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1049" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1049" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1049" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1049" s="2"/>
+      <c r="J1049" s="2"/>
+      <c r="K1049" s="2"/>
+      <c r="L1049" s="2"/>
+      <c r="M1049" s="2"/>
+      <c r="N1049" s="2"/>
+      <c r="O1049" s="2"/>
+      <c r="P1049" s="2"/>
+      <c r="Q1049" s="2"/>
+      <c r="R1049" s="2"/>
+      <c r="S1049" s="2"/>
+      <c r="T1049" s="2"/>
+      <c r="U1049" s="2"/>
+      <c r="V1049" s="2"/>
+      <c r="W1049" s="2"/>
+      <c r="X1049" s="2"/>
+      <c r="Y1049" s="2"/>
+      <c r="Z1049" s="2"/>
+    </row>
+    <row r="1050" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1050" s="1">
+        <v>44963.721655092595</v>
+      </c>
+      <c r="B1050" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1050" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1050" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1050" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1050" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1050" s="2">
+        <v>2</v>
+      </c>
+      <c r="H1050" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1050" s="2"/>
+      <c r="J1050" s="2"/>
+      <c r="K1050" s="2"/>
+      <c r="L1050" s="2"/>
+      <c r="M1050" s="2"/>
+      <c r="N1050" s="2"/>
+      <c r="O1050" s="2"/>
+      <c r="P1050" s="2"/>
+      <c r="Q1050" s="2"/>
+      <c r="R1050" s="2"/>
+      <c r="S1050" s="2"/>
+      <c r="T1050" s="2"/>
+      <c r="U1050" s="2"/>
+      <c r="V1050" s="2"/>
+      <c r="W1050" s="2"/>
+      <c r="X1050" s="2"/>
+      <c r="Y1050" s="2"/>
+      <c r="Z1050" s="2"/>
+    </row>
+    <row r="1051" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1051" s="1">
+        <v>44963.726099537038</v>
+      </c>
+      <c r="B1051" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1051" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1051" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1051" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1051" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1051" s="2">
+        <v>9</v>
+      </c>
+      <c r="H1051" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1051" s="2"/>
+      <c r="J1051" s="2"/>
+      <c r="K1051" s="2"/>
+      <c r="L1051" s="2"/>
+      <c r="M1051" s="2"/>
+      <c r="N1051" s="2"/>
+      <c r="O1051" s="2"/>
+      <c r="P1051" s="2"/>
+      <c r="Q1051" s="2"/>
+      <c r="R1051" s="2"/>
+      <c r="S1051" s="2"/>
+      <c r="T1051" s="2"/>
+      <c r="U1051" s="2"/>
+      <c r="V1051" s="2"/>
+      <c r="W1051" s="2"/>
+      <c r="X1051" s="2"/>
+      <c r="Y1051" s="2"/>
+      <c r="Z1051" s="2"/>
+    </row>
+    <row r="1052" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1052" s="1">
+        <v>44964.567395833335</v>
+      </c>
+      <c r="B1052" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1052" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1052" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1052" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1052" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1052" s="2">
+        <v>3</v>
+      </c>
+      <c r="H1052" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1052" s="2"/>
+      <c r="J1052" s="2"/>
+      <c r="K1052" s="2"/>
+      <c r="L1052" s="2"/>
+      <c r="M1052" s="2"/>
+      <c r="N1052" s="2"/>
+      <c r="O1052" s="2"/>
+      <c r="P1052" s="2"/>
+      <c r="Q1052" s="2"/>
+      <c r="R1052" s="2"/>
+      <c r="S1052" s="2"/>
+      <c r="T1052" s="2"/>
+      <c r="U1052" s="2"/>
+      <c r="V1052" s="2"/>
+      <c r="W1052" s="2"/>
+      <c r="X1052" s="2"/>
+      <c r="Y1052" s="2"/>
+      <c r="Z1052" s="2"/>
+    </row>
+    <row r="1053" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1053" s="1">
+        <v>44965.557222222225</v>
+      </c>
+      <c r="B1053" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1053" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1053" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1053" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1053" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1053" s="2">
+        <v>7</v>
+      </c>
+      <c r="H1053" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1053" s="2"/>
+      <c r="J1053" s="2"/>
+      <c r="K1053" s="2"/>
+      <c r="L1053" s="2"/>
+      <c r="M1053" s="2"/>
+      <c r="N1053" s="2"/>
+      <c r="O1053" s="2"/>
+      <c r="P1053" s="2"/>
+      <c r="Q1053" s="2"/>
+      <c r="R1053" s="2"/>
+      <c r="S1053" s="2"/>
+      <c r="T1053" s="2"/>
+      <c r="U1053" s="2"/>
+      <c r="V1053" s="2"/>
+      <c r="W1053" s="2"/>
+      <c r="X1053" s="2"/>
+      <c r="Y1053" s="2"/>
+      <c r="Z1053" s="2"/>
+    </row>
+    <row r="1054" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1054" s="1">
+        <v>44965.691724537035</v>
+      </c>
+      <c r="B1054" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1054" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1054" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1054" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1054" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1054" s="2">
+        <v>10</v>
+      </c>
+      <c r="H1054" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1054" s="2"/>
+      <c r="J1054" s="2"/>
+      <c r="K1054" s="2"/>
+      <c r="L1054" s="2"/>
+      <c r="M1054" s="2"/>
+      <c r="N1054" s="2"/>
+      <c r="O1054" s="2"/>
+      <c r="P1054" s="2"/>
+      <c r="Q1054" s="2"/>
+      <c r="R1054" s="2"/>
+      <c r="S1054" s="2"/>
+      <c r="T1054" s="2"/>
+      <c r="U1054" s="2"/>
+      <c r="V1054" s="2"/>
+      <c r="W1054" s="2"/>
+      <c r="X1054" s="2"/>
+      <c r="Y1054" s="2"/>
+      <c r="Z1054" s="2"/>
+    </row>
+    <row r="1055" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1055" s="1">
+        <v>44966.683749999997</v>
+      </c>
+      <c r="B1055" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1055" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1055" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1055" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1055" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1055" s="2">
+        <v>5</v>
+      </c>
+      <c r="H1055" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1055" s="2"/>
+      <c r="J1055" s="2"/>
+      <c r="K1055" s="2"/>
+      <c r="L1055" s="2"/>
+      <c r="M1055" s="2"/>
+      <c r="N1055" s="2"/>
+      <c r="O1055" s="2"/>
+      <c r="P1055" s="2"/>
+      <c r="Q1055" s="2"/>
+      <c r="R1055" s="2"/>
+      <c r="S1055" s="2"/>
+      <c r="T1055" s="2"/>
+      <c r="U1055" s="2"/>
+      <c r="V1055" s="2"/>
+      <c r="W1055" s="2"/>
+      <c r="X1055" s="2"/>
+      <c r="Y1055" s="2"/>
+      <c r="Z1055" s="2"/>
+    </row>
+    <row r="1056" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1056" s="1">
+        <v>44966.684131944443</v>
+      </c>
+      <c r="B1056" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1056" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1056" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1056" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1056" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1056" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1056" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1056" s="2"/>
+      <c r="J1056" s="2"/>
+      <c r="K1056" s="2"/>
+      <c r="L1056" s="2"/>
+      <c r="M1056" s="2"/>
+      <c r="N1056" s="2"/>
+      <c r="O1056" s="2"/>
+      <c r="P1056" s="2"/>
+      <c r="Q1056" s="2"/>
+      <c r="R1056" s="2"/>
+      <c r="S1056" s="2"/>
+      <c r="T1056" s="2"/>
+      <c r="U1056" s="2"/>
+      <c r="V1056" s="2"/>
+      <c r="W1056" s="2"/>
+      <c r="X1056" s="2"/>
+      <c r="Y1056" s="2"/>
+      <c r="Z1056" s="2"/>
+    </row>
+    <row r="1057" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1057" s="1">
+        <v>44966.751655092594</v>
+      </c>
+      <c r="B1057" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1057" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1057" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1057" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1057" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1057" s="2">
+        <v>8</v>
+      </c>
+      <c r="H1057" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1057" s="2"/>
+      <c r="J1057" s="2"/>
+      <c r="K1057" s="2"/>
+      <c r="L1057" s="2"/>
+      <c r="M1057" s="2"/>
+      <c r="N1057" s="2"/>
+      <c r="O1057" s="2"/>
+      <c r="P1057" s="2"/>
+      <c r="Q1057" s="2"/>
+      <c r="R1057" s="2"/>
+      <c r="S1057" s="2"/>
+      <c r="T1057" s="2"/>
+      <c r="U1057" s="2"/>
+      <c r="V1057" s="2"/>
+      <c r="W1057" s="2"/>
+      <c r="X1057" s="2"/>
+      <c r="Y1057" s="2"/>
+      <c r="Z1057" s="2"/>
+    </row>
+    <row r="1058" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1058" s="1">
+        <v>44970.533032407409</v>
+      </c>
+      <c r="B1058" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1058" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1058" s="2">
+        <v>9</v>
+      </c>
+      <c r="E1058" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1058" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1058" s="2">
+        <v>11</v>
+      </c>
+      <c r="H1058" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1058" s="2"/>
+      <c r="J1058" s="2"/>
+      <c r="K1058" s="2"/>
+      <c r="L1058" s="2"/>
+      <c r="M1058" s="2"/>
+      <c r="N1058" s="2"/>
+      <c r="O1058" s="2"/>
+      <c r="P1058" s="2"/>
+      <c r="Q1058" s="2"/>
+      <c r="R1058" s="2"/>
+      <c r="S1058" s="2"/>
+      <c r="T1058" s="2"/>
+      <c r="U1058" s="2"/>
+      <c r="V1058" s="2"/>
+      <c r="W1058" s="2"/>
+      <c r="X1058" s="2"/>
+      <c r="Y1058" s="2"/>
+      <c r="Z1058" s="2"/>
+    </row>
+    <row r="1059" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1059" s="1">
+        <v>44970.541921296295</v>
+      </c>
+      <c r="B1059" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1059" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1059" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1059" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1059" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1059" s="2">
+        <v>8</v>
+      </c>
+      <c r="H1059" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1059" s="2"/>
+      <c r="J1059" s="2"/>
+      <c r="K1059" s="2"/>
+      <c r="L1059" s="2"/>
+      <c r="M1059" s="2"/>
+      <c r="N1059" s="2"/>
+      <c r="O1059" s="2"/>
+      <c r="P1059" s="2"/>
+      <c r="Q1059" s="2"/>
+      <c r="R1059" s="2"/>
+      <c r="S1059" s="2"/>
+      <c r="T1059" s="2"/>
+      <c r="U1059" s="2"/>
+      <c r="V1059" s="2"/>
+      <c r="W1059" s="2"/>
+      <c r="X1059" s="2"/>
+      <c r="Y1059" s="2"/>
+      <c r="Z1059" s="2"/>
+    </row>
+    <row r="1060" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1060" s="1">
+        <v>44970.708321759259</v>
+      </c>
+      <c r="B1060" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1060" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1060" s="2">
+        <v>9</v>
+      </c>
+      <c r="E1060" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1060" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1060" s="2">
+        <v>11</v>
+      </c>
+      <c r="H1060" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1060" s="2"/>
+      <c r="J1060" s="2"/>
+      <c r="K1060" s="2"/>
+      <c r="L1060" s="2"/>
+      <c r="M1060" s="2"/>
+      <c r="N1060" s="2"/>
+      <c r="O1060" s="2"/>
+      <c r="P1060" s="2"/>
+      <c r="Q1060" s="2"/>
+      <c r="R1060" s="2"/>
+      <c r="S1060" s="2"/>
+      <c r="T1060" s="2"/>
+      <c r="U1060" s="2"/>
+      <c r="V1060" s="2"/>
+      <c r="W1060" s="2"/>
+      <c r="X1060" s="2"/>
+      <c r="Y1060" s="2"/>
+      <c r="Z1060" s="2"/>
+    </row>
+    <row r="1061" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1061" s="1">
+        <v>44971.521377314813</v>
+      </c>
+      <c r="B1061" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1061" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1061" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1061" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1061" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1061" s="2">
+        <v>3</v>
+      </c>
+      <c r="H1061" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1061" s="2"/>
+      <c r="J1061" s="2"/>
+      <c r="K1061" s="2"/>
+      <c r="L1061" s="2"/>
+      <c r="M1061" s="2"/>
+      <c r="N1061" s="2"/>
+      <c r="O1061" s="2"/>
+      <c r="P1061" s="2"/>
+      <c r="Q1061" s="2"/>
+      <c r="R1061" s="2"/>
+      <c r="S1061" s="2"/>
+      <c r="T1061" s="2"/>
+      <c r="U1061" s="2"/>
+      <c r="V1061" s="2"/>
+      <c r="W1061" s="2"/>
+      <c r="X1061" s="2"/>
+      <c r="Y1061" s="2"/>
+      <c r="Z1061" s="2"/>
+    </row>
+    <row r="1062" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1062" s="1">
+        <v>44971.710509259261</v>
+      </c>
+      <c r="B1062" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1062" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1062" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1062" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1062" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1062" s="2">
+        <v>3</v>
+      </c>
+      <c r="H1062" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1062" s="2"/>
+      <c r="J1062" s="2"/>
+      <c r="K1062" s="2"/>
+      <c r="L1062" s="2"/>
+      <c r="M1062" s="2"/>
+      <c r="N1062" s="2"/>
+      <c r="O1062" s="2"/>
+      <c r="P1062" s="2"/>
+      <c r="Q1062" s="2"/>
+      <c r="R1062" s="2"/>
+      <c r="S1062" s="2"/>
+      <c r="T1062" s="2"/>
+      <c r="U1062" s="2"/>
+      <c r="V1062" s="2"/>
+      <c r="W1062" s="2"/>
+      <c r="X1062" s="2"/>
+      <c r="Y1062" s="2"/>
+      <c r="Z1062" s="2"/>
+    </row>
+    <row r="1063" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1063" s="1">
+        <v>44971.711504629631</v>
+      </c>
+      <c r="B1063" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1063" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1063" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1063" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1063" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1063" s="2">
+        <v>7</v>
+      </c>
+      <c r="H1063" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1063" s="2"/>
+      <c r="J1063" s="2"/>
+      <c r="K1063" s="2"/>
+      <c r="L1063" s="2"/>
+      <c r="M1063" s="2"/>
+      <c r="N1063" s="2"/>
+      <c r="O1063" s="2"/>
+      <c r="P1063" s="2"/>
+      <c r="Q1063" s="2"/>
+      <c r="R1063" s="2"/>
+      <c r="S1063" s="2"/>
+      <c r="T1063" s="2"/>
+      <c r="U1063" s="2"/>
+      <c r="V1063" s="2"/>
+      <c r="W1063" s="2"/>
+      <c r="X1063" s="2"/>
+      <c r="Y1063" s="2"/>
+      <c r="Z1063" s="2"/>
+    </row>
+    <row r="1064" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1064" s="1">
+        <v>44971.712002314816</v>
+      </c>
+      <c r="B1064" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1064" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1064" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1064" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1064" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1064" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1064" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1064" s="2"/>
+      <c r="J1064" s="2"/>
+      <c r="K1064" s="2"/>
+      <c r="L1064" s="2"/>
+      <c r="M1064" s="2"/>
+      <c r="N1064" s="2"/>
+      <c r="O1064" s="2"/>
+      <c r="P1064" s="2"/>
+      <c r="Q1064" s="2"/>
+      <c r="R1064" s="2"/>
+      <c r="S1064" s="2"/>
+      <c r="T1064" s="2"/>
+      <c r="U1064" s="2"/>
+      <c r="V1064" s="2"/>
+      <c r="W1064" s="2"/>
+      <c r="X1064" s="2"/>
+      <c r="Y1064" s="2"/>
+      <c r="Z1064" s="2"/>
+    </row>
+    <row r="1065" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1065" s="1">
+        <v>44971.716400462959</v>
+      </c>
+      <c r="B1065" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1065" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1065" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1065" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1065" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1065" s="2">
+        <v>10</v>
+      </c>
+      <c r="H1065" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1065" s="2"/>
+      <c r="J1065" s="2"/>
+      <c r="K1065" s="2"/>
+      <c r="L1065" s="2"/>
+      <c r="M1065" s="2"/>
+      <c r="N1065" s="2"/>
+      <c r="O1065" s="2"/>
+      <c r="P1065" s="2"/>
+      <c r="Q1065" s="2"/>
+      <c r="R1065" s="2"/>
+      <c r="S1065" s="2"/>
+      <c r="T1065" s="2"/>
+      <c r="U1065" s="2"/>
+      <c r="V1065" s="2"/>
+      <c r="W1065" s="2"/>
+      <c r="X1065" s="2"/>
+      <c r="Y1065" s="2"/>
+      <c r="Z1065" s="2"/>
+    </row>
+    <row r="1066" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1066" s="1">
+        <v>44972.539768518516</v>
+      </c>
+      <c r="B1066" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1066" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1066" s="2">
+        <v>6</v>
+      </c>
+      <c r="E1066" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1066" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1066" s="2">
+        <v>11</v>
+      </c>
+      <c r="H1066" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1066" s="2"/>
+      <c r="J1066" s="2"/>
+      <c r="K1066" s="2"/>
+      <c r="L1066" s="2"/>
+      <c r="M1066" s="2"/>
+      <c r="N1066" s="2"/>
+      <c r="O1066" s="2"/>
+      <c r="P1066" s="2"/>
+      <c r="Q1066" s="2"/>
+      <c r="R1066" s="2"/>
+      <c r="S1066" s="2"/>
+      <c r="T1066" s="2"/>
+      <c r="U1066" s="2"/>
+      <c r="V1066" s="2"/>
+      <c r="W1066" s="2"/>
+      <c r="X1066" s="2"/>
+      <c r="Y1066" s="2"/>
+      <c r="Z1066" s="2"/>
+    </row>
+    <row r="1067" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1067" s="1">
+        <v>44972.54011574074</v>
+      </c>
+      <c r="B1067" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1067" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1067" s="2">
+        <v>6</v>
+      </c>
+      <c r="E1067" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1067" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1067" s="2">
+        <v>11</v>
+      </c>
+      <c r="H1067" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1067" s="2"/>
+      <c r="J1067" s="2"/>
+      <c r="K1067" s="2"/>
+      <c r="L1067" s="2"/>
+      <c r="M1067" s="2"/>
+      <c r="N1067" s="2"/>
+      <c r="O1067" s="2"/>
+      <c r="P1067" s="2"/>
+      <c r="Q1067" s="2"/>
+      <c r="R1067" s="2"/>
+      <c r="S1067" s="2"/>
+      <c r="T1067" s="2"/>
+      <c r="U1067" s="2"/>
+      <c r="V1067" s="2"/>
+      <c r="W1067" s="2"/>
+      <c r="X1067" s="2"/>
+      <c r="Y1067" s="2"/>
+      <c r="Z1067" s="2"/>
+    </row>
+    <row r="1068" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1068" s="1">
+        <v>44972.549444444441</v>
+      </c>
+      <c r="B1068" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1068" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1068" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1068" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1068" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1068" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1068" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1068" s="2"/>
+      <c r="J1068" s="2"/>
+      <c r="K1068" s="2"/>
+      <c r="L1068" s="2"/>
+      <c r="M1068" s="2"/>
+      <c r="N1068" s="2"/>
+      <c r="O1068" s="2"/>
+      <c r="P1068" s="2"/>
+      <c r="Q1068" s="2"/>
+      <c r="R1068" s="2"/>
+      <c r="S1068" s="2"/>
+      <c r="T1068" s="2"/>
+      <c r="U1068" s="2"/>
+      <c r="V1068" s="2"/>
+      <c r="W1068" s="2"/>
+      <c r="X1068" s="2"/>
+      <c r="Y1068" s="2"/>
+      <c r="Z1068" s="2"/>
+    </row>
+    <row r="1069" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1069" s="1">
+        <v>44972.684328703705</v>
+      </c>
+      <c r="B1069" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1069" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1069" s="2">
+        <v>9</v>
+      </c>
+      <c r="E1069" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1069" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1069" s="2">
+        <v>11</v>
+      </c>
+      <c r="H1069" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1069" s="2"/>
+      <c r="J1069" s="2"/>
+      <c r="K1069" s="2"/>
+      <c r="L1069" s="2"/>
+      <c r="M1069" s="2"/>
+      <c r="N1069" s="2"/>
+      <c r="O1069" s="2"/>
+      <c r="P1069" s="2"/>
+      <c r="Q1069" s="2"/>
+      <c r="R1069" s="2"/>
+      <c r="S1069" s="2"/>
+      <c r="T1069" s="2"/>
+      <c r="U1069" s="2"/>
+      <c r="V1069" s="2"/>
+      <c r="W1069" s="2"/>
+      <c r="X1069" s="2"/>
+      <c r="Y1069" s="2"/>
+      <c r="Z1069" s="2"/>
+    </row>
+    <row r="1070" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1070" s="1">
+        <v>44973.53802083333</v>
+      </c>
+      <c r="B1070" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1070" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1070" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1070" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1070" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1070" s="2">
+        <v>3</v>
+      </c>
+      <c r="H1070" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1070" s="2"/>
+      <c r="J1070" s="2"/>
+      <c r="K1070" s="2"/>
+      <c r="L1070" s="2"/>
+      <c r="M1070" s="2"/>
+      <c r="N1070" s="2"/>
+      <c r="O1070" s="2"/>
+      <c r="P1070" s="2"/>
+      <c r="Q1070" s="2"/>
+      <c r="R1070" s="2"/>
+      <c r="S1070" s="2"/>
+      <c r="T1070" s="2"/>
+      <c r="U1070" s="2"/>
+      <c r="V1070" s="2"/>
+      <c r="W1070" s="2"/>
+      <c r="X1070" s="2"/>
+      <c r="Y1070" s="2"/>
+      <c r="Z1070" s="2"/>
+    </row>
+    <row r="1071" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1071" s="1">
+        <v>44973.546701388892</v>
+      </c>
+      <c r="B1071" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1071" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1071" s="2">
+        <v>8</v>
+      </c>
+      <c r="E1071" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1071" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1071" s="2">
+        <v>11</v>
+      </c>
+      <c r="H1071" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1071" s="2"/>
+      <c r="J1071" s="2"/>
+      <c r="K1071" s="2"/>
+      <c r="L1071" s="2"/>
+      <c r="M1071" s="2"/>
+      <c r="N1071" s="2"/>
+      <c r="O1071" s="2"/>
+      <c r="P1071" s="2"/>
+      <c r="Q1071" s="2"/>
+      <c r="R1071" s="2"/>
+      <c r="S1071" s="2"/>
+      <c r="T1071" s="2"/>
+      <c r="U1071" s="2"/>
+      <c r="V1071" s="2"/>
+      <c r="W1071" s="2"/>
+      <c r="X1071" s="2"/>
+      <c r="Y1071" s="2"/>
+      <c r="Z1071" s="2"/>
+    </row>
+    <row r="1072" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1072" s="1">
+        <v>44973.553078703706</v>
+      </c>
+      <c r="B1072" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1072" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1072" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1072" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1072" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1072" s="2">
+        <v>4</v>
+      </c>
+      <c r="H1072" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1072" s="2"/>
+      <c r="J1072" s="2"/>
+      <c r="K1072" s="2"/>
+      <c r="L1072" s="2"/>
+      <c r="M1072" s="2"/>
+      <c r="N1072" s="2"/>
+      <c r="O1072" s="2"/>
+      <c r="P1072" s="2"/>
+      <c r="Q1072" s="2"/>
+      <c r="R1072" s="2"/>
+      <c r="S1072" s="2"/>
+      <c r="T1072" s="2"/>
+      <c r="U1072" s="2"/>
+      <c r="V1072" s="2"/>
+      <c r="W1072" s="2"/>
+      <c r="X1072" s="2"/>
+      <c r="Y1072" s="2"/>
+      <c r="Z1072" s="2"/>
+    </row>
+    <row r="1073" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1073" s="1">
+        <v>44977.539398148147</v>
+      </c>
+      <c r="B1073" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1073" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1073" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1073" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1073" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1073" s="2">
+        <v>3</v>
+      </c>
+      <c r="H1073" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1073" s="2"/>
+      <c r="J1073" s="2"/>
+      <c r="K1073" s="2"/>
+      <c r="L1073" s="2"/>
+      <c r="M1073" s="2"/>
+      <c r="N1073" s="2"/>
+      <c r="O1073" s="2"/>
+      <c r="P1073" s="2"/>
+      <c r="Q1073" s="2"/>
+      <c r="R1073" s="2"/>
+      <c r="S1073" s="2"/>
+      <c r="T1073" s="2"/>
+      <c r="U1073" s="2"/>
+      <c r="V1073" s="2"/>
+      <c r="W1073" s="2"/>
+      <c r="X1073" s="2"/>
+      <c r="Y1073" s="2"/>
+      <c r="Z1073" s="2"/>
+    </row>
+    <row r="1074" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1074" s="1">
+        <v>44977.67465277778</v>
+      </c>
+      <c r="B1074" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1074" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1074" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1074" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1074" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1074" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1074" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1074" s="2"/>
+      <c r="J1074" s="2"/>
+      <c r="K1074" s="2"/>
+      <c r="L1074" s="2"/>
+      <c r="M1074" s="2"/>
+      <c r="N1074" s="2"/>
+      <c r="O1074" s="2"/>
+      <c r="P1074" s="2"/>
+      <c r="Q1074" s="2"/>
+      <c r="R1074" s="2"/>
+      <c r="S1074" s="2"/>
+      <c r="T1074" s="2"/>
+      <c r="U1074" s="2"/>
+      <c r="V1074" s="2"/>
+      <c r="W1074" s="2"/>
+      <c r="X1074" s="2"/>
+      <c r="Y1074" s="2"/>
+      <c r="Z1074" s="2"/>
+    </row>
+    <row r="1075" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1075" s="1">
+        <v>44977.722812499997</v>
+      </c>
+      <c r="B1075" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1075" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1075" s="2">
+        <v>5</v>
+      </c>
+      <c r="E1075" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1075" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1075" s="2">
+        <v>11</v>
+      </c>
+      <c r="H1075" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1075" s="2"/>
+      <c r="J1075" s="2"/>
+      <c r="K1075" s="2"/>
+      <c r="L1075" s="2"/>
+      <c r="M1075" s="2"/>
+      <c r="N1075" s="2"/>
+      <c r="O1075" s="2"/>
+      <c r="P1075" s="2"/>
+      <c r="Q1075" s="2"/>
+      <c r="R1075" s="2"/>
+      <c r="S1075" s="2"/>
+      <c r="T1075" s="2"/>
+      <c r="U1075" s="2"/>
+      <c r="V1075" s="2"/>
+      <c r="W1075" s="2"/>
+      <c r="X1075" s="2"/>
+      <c r="Y1075" s="2"/>
+      <c r="Z1075" s="2"/>
+    </row>
+    <row r="1076" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1076" s="1">
+        <v>44977.766585648147</v>
+      </c>
+      <c r="B1076" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1076" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1076" s="2">
+        <v>10</v>
+      </c>
+      <c r="E1076" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1076" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1076" s="2">
+        <v>11</v>
+      </c>
+      <c r="H1076" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1076" s="2"/>
+      <c r="J1076" s="2"/>
+      <c r="K1076" s="2"/>
+      <c r="L1076" s="2"/>
+      <c r="M1076" s="2"/>
+      <c r="N1076" s="2"/>
+      <c r="O1076" s="2"/>
+      <c r="P1076" s="2"/>
+      <c r="Q1076" s="2"/>
+      <c r="R1076" s="2"/>
+      <c r="S1076" s="2"/>
+      <c r="T1076" s="2"/>
+      <c r="U1076" s="2"/>
+      <c r="V1076" s="2"/>
+      <c r="W1076" s="2"/>
+      <c r="X1076" s="2"/>
+      <c r="Y1076" s="2"/>
+      <c r="Z1076" s="2"/>
+    </row>
+    <row r="1077" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1077" s="1">
+        <v>44978.384131944447</v>
+      </c>
+      <c r="B1077" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1077" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1077" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1077" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1077" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1077" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1077" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1077" s="2"/>
+      <c r="J1077" s="2"/>
+      <c r="K1077" s="2"/>
+      <c r="L1077" s="2"/>
+      <c r="M1077" s="2"/>
+      <c r="N1077" s="2"/>
+      <c r="O1077" s="2"/>
+      <c r="P1077" s="2"/>
+      <c r="Q1077" s="2"/>
+      <c r="R1077" s="2"/>
+      <c r="S1077" s="2"/>
+      <c r="T1077" s="2"/>
+      <c r="U1077" s="2"/>
+      <c r="V1077" s="2"/>
+      <c r="W1077" s="2"/>
+      <c r="X1077" s="2"/>
+      <c r="Y1077" s="2"/>
+      <c r="Z1077" s="2"/>
+    </row>
+    <row r="1078" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1078" s="1">
+        <v>44978.544039351851</v>
+      </c>
+      <c r="B1078" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1078" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1078" s="2">
+        <v>10</v>
+      </c>
+      <c r="E1078" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1078" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1078" s="2">
+        <v>11</v>
+      </c>
+      <c r="H1078" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1078" s="2"/>
+      <c r="J1078" s="2"/>
+      <c r="K1078" s="2"/>
+      <c r="L1078" s="2"/>
+      <c r="M1078" s="2"/>
+      <c r="N1078" s="2"/>
+      <c r="O1078" s="2"/>
+      <c r="P1078" s="2"/>
+      <c r="Q1078" s="2"/>
+      <c r="R1078" s="2"/>
+      <c r="S1078" s="2"/>
+      <c r="T1078" s="2"/>
+      <c r="U1078" s="2"/>
+      <c r="V1078" s="2"/>
+      <c r="W1078" s="2"/>
+      <c r="X1078" s="2"/>
+      <c r="Y1078" s="2"/>
+      <c r="Z1078" s="2"/>
+    </row>
+    <row r="1079" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1079" s="1">
+        <v>44978.557673611111</v>
+      </c>
+      <c r="B1079" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1079" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1079" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1079" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1079" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1079" s="2">
+        <v>10</v>
+      </c>
+      <c r="H1079" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1079" s="2"/>
+      <c r="J1079" s="2"/>
+      <c r="K1079" s="2"/>
+      <c r="L1079" s="2"/>
+      <c r="M1079" s="2"/>
+      <c r="N1079" s="2"/>
+      <c r="O1079" s="2"/>
+      <c r="P1079" s="2"/>
+      <c r="Q1079" s="2"/>
+      <c r="R1079" s="2"/>
+      <c r="S1079" s="2"/>
+      <c r="T1079" s="2"/>
+      <c r="U1079" s="2"/>
+      <c r="V1079" s="2"/>
+      <c r="W1079" s="2"/>
+      <c r="X1079" s="2"/>
+      <c r="Y1079" s="2"/>
+      <c r="Z1079" s="2"/>
+    </row>
+    <row r="1080" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1080" s="1">
+        <v>44978.706319444442</v>
+      </c>
+      <c r="B1080" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1080" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1080" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1080" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1080" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1080" s="2">
+        <v>10</v>
+      </c>
+      <c r="H1080" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1080" s="2"/>
+      <c r="J1080" s="2"/>
+      <c r="K1080" s="2"/>
+      <c r="L1080" s="2"/>
+      <c r="M1080" s="2"/>
+      <c r="N1080" s="2"/>
+      <c r="O1080" s="2"/>
+      <c r="P1080" s="2"/>
+      <c r="Q1080" s="2"/>
+      <c r="R1080" s="2"/>
+      <c r="S1080" s="2"/>
+      <c r="T1080" s="2"/>
+      <c r="U1080" s="2"/>
+      <c r="V1080" s="2"/>
+      <c r="W1080" s="2"/>
+      <c r="X1080" s="2"/>
+      <c r="Y1080" s="2"/>
+      <c r="Z1080" s="2"/>
+    </row>
+    <row r="1081" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1081" s="1">
+        <v>44979.552025462966</v>
+      </c>
+      <c r="B1081" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1081" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1081" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1081" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1081" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1081" s="2">
+        <v>5</v>
+      </c>
+      <c r="H1081" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1081" s="2"/>
+      <c r="J1081" s="2"/>
+      <c r="K1081" s="2"/>
+      <c r="L1081" s="2"/>
+      <c r="M1081" s="2"/>
+      <c r="N1081" s="2"/>
+      <c r="O1081" s="2"/>
+      <c r="P1081" s="2"/>
+      <c r="Q1081" s="2"/>
+      <c r="R1081" s="2"/>
+      <c r="S1081" s="2"/>
+      <c r="T1081" s="2"/>
+      <c r="U1081" s="2"/>
+      <c r="V1081" s="2"/>
+      <c r="W1081" s="2"/>
+      <c r="X1081" s="2"/>
+      <c r="Y1081" s="2"/>
+      <c r="Z1081" s="2"/>
+    </row>
+    <row r="1082" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1082" s="1">
+        <v>44979.762685185182</v>
+      </c>
+      <c r="B1082" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1082" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1082" s="2">
+        <v>7</v>
+      </c>
+      <c r="E1082" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1082" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1082" s="2">
+        <v>11</v>
+      </c>
+      <c r="H1082" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1082" s="2"/>
+      <c r="J1082" s="2"/>
+      <c r="K1082" s="2"/>
+      <c r="L1082" s="2"/>
+      <c r="M1082" s="2"/>
+      <c r="N1082" s="2"/>
+      <c r="O1082" s="2"/>
+      <c r="P1082" s="2"/>
+      <c r="Q1082" s="2"/>
+      <c r="R1082" s="2"/>
+      <c r="S1082" s="2"/>
+      <c r="T1082" s="2"/>
+      <c r="U1082" s="2"/>
+      <c r="V1082" s="2"/>
+      <c r="W1082" s="2"/>
+      <c r="X1082" s="2"/>
+      <c r="Y1082" s="2"/>
+      <c r="Z1082" s="2"/>
+    </row>
+    <row r="1083" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1083" s="1">
+        <v>44979.76394675926</v>
+      </c>
+      <c r="B1083" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1083" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1083" s="2">
+        <v>6</v>
+      </c>
+      <c r="E1083" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1083" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1083" s="2">
+        <v>11</v>
+      </c>
+      <c r="H1083" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1083" s="2"/>
+      <c r="J1083" s="2"/>
+      <c r="K1083" s="2"/>
+      <c r="L1083" s="2"/>
+      <c r="M1083" s="2"/>
+      <c r="N1083" s="2"/>
+      <c r="O1083" s="2"/>
+      <c r="P1083" s="2"/>
+      <c r="Q1083" s="2"/>
+      <c r="R1083" s="2"/>
+      <c r="S1083" s="2"/>
+      <c r="T1083" s="2"/>
+      <c r="U1083" s="2"/>
+      <c r="V1083" s="2"/>
+      <c r="W1083" s="2"/>
+      <c r="X1083" s="2"/>
+      <c r="Y1083" s="2"/>
+      <c r="Z1083" s="2"/>
+    </row>
+    <row r="1084" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1084" s="1">
+        <v>44979.764398148145</v>
+      </c>
+      <c r="B1084" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1084" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1084" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1084" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1084" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1084" s="2">
+        <v>3</v>
+      </c>
+      <c r="H1084" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1084" s="2"/>
+      <c r="J1084" s="2"/>
+      <c r="K1084" s="2"/>
+      <c r="L1084" s="2"/>
+      <c r="M1084" s="2"/>
+      <c r="N1084" s="2"/>
+      <c r="O1084" s="2"/>
+      <c r="P1084" s="2"/>
+      <c r="Q1084" s="2"/>
+      <c r="R1084" s="2"/>
+      <c r="S1084" s="2"/>
+      <c r="T1084" s="2"/>
+      <c r="U1084" s="2"/>
+      <c r="V1084" s="2"/>
+      <c r="W1084" s="2"/>
+      <c r="X1084" s="2"/>
+      <c r="Y1084" s="2"/>
+      <c r="Z1084" s="2"/>
+    </row>
+    <row r="1085" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1085" s="1">
+        <v>44980.54991898148</v>
+      </c>
+      <c r="B1085" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1085" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1085" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1085" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1085" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1085" s="2">
+        <v>3</v>
+      </c>
+      <c r="H1085" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1085" s="2"/>
+      <c r="J1085" s="2"/>
+      <c r="K1085" s="2"/>
+      <c r="L1085" s="2"/>
+      <c r="M1085" s="2"/>
+      <c r="N1085" s="2"/>
+      <c r="O1085" s="2"/>
+      <c r="P1085" s="2"/>
+      <c r="Q1085" s="2"/>
+      <c r="R1085" s="2"/>
+      <c r="S1085" s="2"/>
+      <c r="T1085" s="2"/>
+      <c r="U1085" s="2"/>
+      <c r="V1085" s="2"/>
+      <c r="W1085" s="2"/>
+      <c r="X1085" s="2"/>
+      <c r="Y1085" s="2"/>
+      <c r="Z1085" s="2"/>
+    </row>
+    <row r="1086" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1086" s="1">
+        <v>44980.657870370371</v>
+      </c>
+      <c r="B1086" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1086" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1086" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1086" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1086" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1086" s="2">
+        <v>8</v>
+      </c>
+      <c r="H1086" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1086" s="2"/>
+      <c r="J1086" s="2"/>
+      <c r="K1086" s="2"/>
+      <c r="L1086" s="2"/>
+      <c r="M1086" s="2"/>
+      <c r="N1086" s="2"/>
+      <c r="O1086" s="2"/>
+      <c r="P1086" s="2"/>
+      <c r="Q1086" s="2"/>
+      <c r="R1086" s="2"/>
+      <c r="S1086" s="2"/>
+      <c r="T1086" s="2"/>
+      <c r="U1086" s="2"/>
+      <c r="V1086" s="2"/>
+      <c r="W1086" s="2"/>
+      <c r="X1086" s="2"/>
+      <c r="Y1086" s="2"/>
+      <c r="Z1086" s="2"/>
+    </row>
+    <row r="1087" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1087" s="1">
+        <v>44980.695370370369</v>
+      </c>
+      <c r="B1087" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1087" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1087" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1087" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1087" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1087" s="2">
+        <v>8</v>
+      </c>
+      <c r="H1087" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1087" s="2"/>
+      <c r="J1087" s="2"/>
+      <c r="K1087" s="2"/>
+      <c r="L1087" s="2"/>
+      <c r="M1087" s="2"/>
+      <c r="N1087" s="2"/>
+      <c r="O1087" s="2"/>
+      <c r="P1087" s="2"/>
+      <c r="Q1087" s="2"/>
+      <c r="R1087" s="2"/>
+      <c r="S1087" s="2"/>
+      <c r="T1087" s="2"/>
+      <c r="U1087" s="2"/>
+      <c r="V1087" s="2"/>
+      <c r="W1087" s="2"/>
+      <c r="X1087" s="2"/>
+      <c r="Y1087" s="2"/>
+      <c r="Z1087" s="2"/>
+    </row>
+    <row r="1088" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1088" s="1">
+        <v>44980.695833333331</v>
+      </c>
+      <c r="B1088" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1088" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1088" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1088" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1088" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1088" s="2">
+        <v>4</v>
+      </c>
+      <c r="H1088" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1088" s="2"/>
+      <c r="J1088" s="2"/>
+      <c r="K1088" s="2"/>
+      <c r="L1088" s="2"/>
+      <c r="M1088" s="2"/>
+      <c r="N1088" s="2"/>
+      <c r="O1088" s="2"/>
+      <c r="P1088" s="2"/>
+      <c r="Q1088" s="2"/>
+      <c r="R1088" s="2"/>
+      <c r="S1088" s="2"/>
+      <c r="T1088" s="2"/>
+      <c r="U1088" s="2"/>
+      <c r="V1088" s="2"/>
+      <c r="W1088" s="2"/>
+      <c r="X1088" s="2"/>
+      <c r="Y1088" s="2"/>
+      <c r="Z1088" s="2"/>
+    </row>
+    <row r="1089" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1089" s="1">
+        <v>44980.699837962966</v>
+      </c>
+      <c r="B1089" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1089" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1089" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1089" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1089" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1089" s="2">
+        <v>4</v>
+      </c>
+      <c r="H1089" t="str">
+        <f t="shared" si="16"/>
+        <v>ok</v>
+      </c>
+      <c r="I1089" s="2"/>
+      <c r="J1089" s="2"/>
+      <c r="K1089" s="2"/>
+      <c r="L1089" s="2"/>
+      <c r="M1089" s="2"/>
+      <c r="N1089" s="2"/>
+      <c r="O1089" s="2"/>
+      <c r="P1089" s="2"/>
+      <c r="Q1089" s="2"/>
+      <c r="R1089" s="2"/>
+      <c r="S1089" s="2"/>
+      <c r="T1089" s="2"/>
+      <c r="U1089" s="2"/>
+      <c r="V1089" s="2"/>
+      <c r="W1089" s="2"/>
+      <c r="X1089" s="2"/>
+      <c r="Y1089" s="2"/>
+      <c r="Z1089" s="2"/>
+    </row>
+    <row r="1090" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1090" s="1">
+        <v>44980.706226851849</v>
+      </c>
+      <c r="B1090" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1090" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1090" s="2">
+        <v>6</v>
+      </c>
+      <c r="E1090" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1090" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1090" s="2">
+        <v>11</v>
+      </c>
+      <c r="H1090" t="str">
+        <f t="shared" ref="H1090:H1095" si="17">IF(D1090=G1090,"error","ok")</f>
+        <v>ok</v>
+      </c>
+      <c r="I1090" s="2"/>
+      <c r="J1090" s="2"/>
+      <c r="K1090" s="2"/>
+      <c r="L1090" s="2"/>
+      <c r="M1090" s="2"/>
+      <c r="N1090" s="2"/>
+      <c r="O1090" s="2"/>
+      <c r="P1090" s="2"/>
+      <c r="Q1090" s="2"/>
+      <c r="R1090" s="2"/>
+      <c r="S1090" s="2"/>
+      <c r="T1090" s="2"/>
+      <c r="U1090" s="2"/>
+      <c r="V1090" s="2"/>
+      <c r="W1090" s="2"/>
+      <c r="X1090" s="2"/>
+      <c r="Y1090" s="2"/>
+      <c r="Z1090" s="2"/>
+    </row>
+    <row r="1091" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1091" s="1">
+        <v>44980.717314814814</v>
+      </c>
+      <c r="B1091" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1091" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1091" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1091" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1091" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1091" s="2">
+        <v>10</v>
+      </c>
+      <c r="H1091" t="str">
+        <f t="shared" si="17"/>
+        <v>ok</v>
+      </c>
+      <c r="I1091" s="2"/>
+      <c r="J1091" s="2"/>
+      <c r="K1091" s="2"/>
+      <c r="L1091" s="2"/>
+      <c r="M1091" s="2"/>
+      <c r="N1091" s="2"/>
+      <c r="O1091" s="2"/>
+      <c r="P1091" s="2"/>
+      <c r="Q1091" s="2"/>
+      <c r="R1091" s="2"/>
+      <c r="S1091" s="2"/>
+      <c r="T1091" s="2"/>
+      <c r="U1091" s="2"/>
+      <c r="V1091" s="2"/>
+      <c r="W1091" s="2"/>
+      <c r="X1091" s="2"/>
+      <c r="Y1091" s="2"/>
+      <c r="Z1091" s="2"/>
+    </row>
+    <row r="1092" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1092" s="1">
+        <v>44984.695659722223</v>
+      </c>
+      <c r="B1092" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1092" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1092" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1092" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1092" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1092" s="2">
+        <v>4</v>
+      </c>
+      <c r="H1092" t="str">
+        <f t="shared" si="17"/>
+        <v>ok</v>
+      </c>
+      <c r="I1092" s="2"/>
+      <c r="J1092" s="2"/>
+      <c r="K1092" s="2"/>
+      <c r="L1092" s="2"/>
+      <c r="M1092" s="2"/>
+      <c r="N1092" s="2"/>
+      <c r="O1092" s="2"/>
+      <c r="P1092" s="2"/>
+      <c r="Q1092" s="2"/>
+      <c r="R1092" s="2"/>
+      <c r="S1092" s="2"/>
+      <c r="T1092" s="2"/>
+      <c r="U1092" s="2"/>
+      <c r="V1092" s="2"/>
+      <c r="W1092" s="2"/>
+      <c r="X1092" s="2"/>
+      <c r="Y1092" s="2"/>
+      <c r="Z1092" s="2"/>
+    </row>
+    <row r="1093" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1093" s="1">
+        <v>44984.723078703704</v>
+      </c>
+      <c r="B1093" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1093" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1093" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1093" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1093" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1093" s="2">
+        <v>7</v>
+      </c>
+      <c r="H1093" t="str">
+        <f t="shared" si="17"/>
+        <v>ok</v>
+      </c>
+      <c r="I1093" s="2"/>
+      <c r="J1093" s="2"/>
+      <c r="K1093" s="2"/>
+      <c r="L1093" s="2"/>
+      <c r="M1093" s="2"/>
+      <c r="N1093" s="2"/>
+      <c r="O1093" s="2"/>
+      <c r="P1093" s="2"/>
+      <c r="Q1093" s="2"/>
+      <c r="R1093" s="2"/>
+      <c r="S1093" s="2"/>
+      <c r="T1093" s="2"/>
+      <c r="U1093" s="2"/>
+      <c r="V1093" s="2"/>
+      <c r="W1093" s="2"/>
+      <c r="X1093" s="2"/>
+      <c r="Y1093" s="2"/>
+      <c r="Z1093" s="2"/>
+    </row>
+    <row r="1094" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1094" s="1">
+        <v>44985.546342592592</v>
+      </c>
+      <c r="B1094" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1094" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1094" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1094" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1094" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1094" s="2">
+        <v>10</v>
+      </c>
+      <c r="H1094" t="str">
+        <f t="shared" si="17"/>
+        <v>ok</v>
+      </c>
+      <c r="I1094" s="2"/>
+      <c r="J1094" s="2"/>
+      <c r="K1094" s="2"/>
+      <c r="L1094" s="2"/>
+      <c r="M1094" s="2"/>
+      <c r="N1094" s="2"/>
+      <c r="O1094" s="2"/>
+      <c r="P1094" s="2"/>
+      <c r="Q1094" s="2"/>
+      <c r="R1094" s="2"/>
+      <c r="S1094" s="2"/>
+      <c r="T1094" s="2"/>
+      <c r="U1094" s="2"/>
+      <c r="V1094" s="2"/>
+      <c r="W1094" s="2"/>
+      <c r="X1094" s="2"/>
+      <c r="Y1094" s="2"/>
+      <c r="Z1094" s="2"/>
+    </row>
+    <row r="1095" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1095" s="1">
+        <v>44985.546354166669</v>
+      </c>
+      <c r="B1095" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1095" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1095" s="2">
+        <v>11</v>
+      </c>
+      <c r="E1095" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1095" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1095" s="2">
+        <v>2</v>
+      </c>
+      <c r="H1095" t="str">
+        <f t="shared" si="17"/>
+        <v>ok</v>
+      </c>
+      <c r="I1095" s="2"/>
+      <c r="J1095" s="2"/>
+      <c r="K1095" s="2"/>
+      <c r="L1095" s="2"/>
+      <c r="M1095" s="2"/>
+      <c r="N1095" s="2"/>
+      <c r="O1095" s="2"/>
+      <c r="P1095" s="2"/>
+      <c r="Q1095" s="2"/>
+      <c r="R1095" s="2"/>
+      <c r="S1095" s="2"/>
+      <c r="T1095" s="2"/>
+      <c r="U1095" s="2"/>
+      <c r="V1095" s="2"/>
+      <c r="W1095" s="2"/>
+      <c r="X1095" s="2"/>
+      <c r="Y1095" s="2"/>
+    </row>
+    <row r="1096" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1096" s="2"/>
       <c r="B1096" s="2"/>
       <c r="C1096" s="2"/>
@@ -29061,7 +31079,7 @@
       <c r="F1096" s="2"/>
       <c r="G1096" s="2"/>
     </row>
-    <row r="1097" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1097" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1097" s="2"/>
       <c r="B1097" s="2"/>
       <c r="C1097" s="2"/>
@@ -29070,7 +31088,7 @@
       <c r="F1097" s="2"/>
       <c r="G1097" s="2"/>
     </row>
-    <row r="1098" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1098" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1098" s="2"/>
       <c r="B1098" s="2"/>
       <c r="C1098" s="2"/>
@@ -29079,7 +31097,7 @@
       <c r="F1098" s="2"/>
       <c r="G1098" s="2"/>
     </row>
-    <row r="1099" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1099" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1099" s="2"/>
       <c r="B1099" s="2"/>
       <c r="C1099" s="2"/>
@@ -29088,7 +31106,7 @@
       <c r="F1099" s="2"/>
       <c r="G1099" s="2"/>
     </row>
-    <row r="1100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1100" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1100" s="2"/>
       <c r="B1100" s="2"/>
       <c r="C1100" s="2"/>
@@ -29097,7 +31115,7 @@
       <c r="F1100" s="2"/>
       <c r="G1100" s="2"/>
     </row>
-    <row r="1101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1101" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1101" s="2"/>
       <c r="B1101" s="2"/>
       <c r="C1101" s="2"/>
@@ -29106,7 +31124,7 @@
       <c r="F1101" s="2"/>
       <c r="G1101" s="2"/>
     </row>
-    <row r="1102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1102" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1102" s="2"/>
       <c r="B1102" s="2"/>
       <c r="C1102" s="2"/>
@@ -29115,7 +31133,7 @@
       <c r="F1102" s="2"/>
       <c r="G1102" s="2"/>
     </row>
-    <row r="1103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1103" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1103" s="2"/>
       <c r="B1103" s="2"/>
       <c r="C1103" s="2"/>
@@ -29124,7 +31142,7 @@
       <c r="F1103" s="2"/>
       <c r="G1103" s="2"/>
     </row>
-    <row r="1104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1104" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1104" s="2"/>
       <c r="B1104" s="2"/>
       <c r="C1104" s="2"/>
@@ -32731,27 +34749,9 @@
       <c r="D1504" s="2"/>
       <c r="E1504" s="2"/>
       <c r="F1504" s="2"/>
-      <c r="G1504" s="2"/>
-    </row>
-    <row r="1505" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1505" s="2"/>
-      <c r="B1505" s="2"/>
-      <c r="C1505" s="2"/>
-      <c r="D1505" s="2"/>
-      <c r="E1505" s="2"/>
-      <c r="F1505" s="2"/>
-      <c r="G1505" s="2"/>
-    </row>
-    <row r="1506" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1506" s="2"/>
-      <c r="B1506" s="2"/>
-      <c r="C1506" s="2"/>
-      <c r="D1506" s="2"/>
-      <c r="E1506" s="2"/>
-      <c r="F1506" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1048576">
+  <conditionalFormatting sqref="D1:D1038 D1096:D1048576">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"g1"</formula>
     </cfRule>

</xml_diff>

<commit_message>
adding redirection to home page
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lazarekolebka/Documents/GitHub/baby-foot-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21D5B28-A385-B540-B12A-B4E1F4BC12F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F136FD4-C0BD-FD41-8D2A-9F240A50CDBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16520" xr2:uid="{3047FE35-D3D7-B143-93A4-201EEA00FB6B}"/>
   </bookViews>
@@ -471,7 +471,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8CBF0B-E51F-9843-B378-4476707EC7F4}">
   <dimension ref="A1:Z1504"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A736" zoomScale="112" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="112" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:J8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>